<commit_message>
computer about to die
</commit_message>
<xml_diff>
--- a/python training environment/cRIO timing and SNR.xlsx
+++ b/python training environment/cRIO timing and SNR.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dncob\Documents\GitHub\Real-time-LSTM\python training environment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A07B40E-0D53-4470-9804-73B9B49C5418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91839245-B2B2-4B8F-B2DA-6A5D9CAFFD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3DFDAE7D-E760-451F-B681-94403AFEABDB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{3DFDAE7D-E760-451F-B681-94403AFEABDB}"/>
   </bookViews>
   <sheets>
     <sheet name="experimental timing" sheetId="1" r:id="rId1"/>
     <sheet name="SNR table" sheetId="2" r:id="rId2"/>
+    <sheet name="Bigger SNR Tables" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
   <si>
     <t>analog read</t>
   </si>
@@ -123,6 +124,9 @@
   </si>
   <si>
     <t>Validation Profile:</t>
+  </si>
+  <si>
+    <t>1 Cell</t>
   </si>
 </sst>
 </file>
@@ -171,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -181,6 +185,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1773,8 +1778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7945617-BC65-4E48-B28B-121AF4036495}">
   <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1:Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2417,4 +2422,461 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74CB922C-46C9-4822-8489-8BECDA10DEAF}">
+  <dimension ref="A1:AN10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AT17" sqref="AT17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" customWidth="1"/>
+    <col min="17" max="17" width="12.5546875" customWidth="1"/>
+    <col min="30" max="30" width="13.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1">
+        <v>29.143000000000001</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2">
+        <v>3.49E-2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2">
+        <v>40</v>
+      </c>
+      <c r="F2">
+        <v>35</v>
+      </c>
+      <c r="G2">
+        <v>30</v>
+      </c>
+      <c r="H2">
+        <v>25</v>
+      </c>
+      <c r="I2">
+        <v>20</v>
+      </c>
+      <c r="J2">
+        <v>18</v>
+      </c>
+      <c r="K2">
+        <v>15</v>
+      </c>
+      <c r="L2">
+        <v>12</v>
+      </c>
+      <c r="M2">
+        <v>10</v>
+      </c>
+      <c r="N2">
+        <v>8</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2">
+        <v>40</v>
+      </c>
+      <c r="S2">
+        <v>35</v>
+      </c>
+      <c r="T2">
+        <v>30</v>
+      </c>
+      <c r="U2">
+        <v>25</v>
+      </c>
+      <c r="V2">
+        <v>20</v>
+      </c>
+      <c r="W2">
+        <v>18</v>
+      </c>
+      <c r="X2">
+        <v>15</v>
+      </c>
+      <c r="Y2">
+        <v>12</v>
+      </c>
+      <c r="Z2">
+        <v>10</v>
+      </c>
+      <c r="AA2">
+        <v>8</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE2">
+        <v>40</v>
+      </c>
+      <c r="AF2">
+        <v>35</v>
+      </c>
+      <c r="AG2">
+        <v>30</v>
+      </c>
+      <c r="AH2">
+        <v>25</v>
+      </c>
+      <c r="AI2">
+        <v>20</v>
+      </c>
+      <c r="AJ2">
+        <v>18</v>
+      </c>
+      <c r="AK2">
+        <v>15</v>
+      </c>
+      <c r="AL2">
+        <v>12</v>
+      </c>
+      <c r="AM2">
+        <v>10</v>
+      </c>
+      <c r="AN2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>0.50060000000000004</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3">
+        <f>$B$1+$B$2*(68*E2+4*E2^2)+$B$3*5*E2</f>
+        <v>447.55100000000004</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:N3" si="0">$B$1+$B$2*(68*F2+4*F2^2)+$B$3*5*F2</f>
+        <v>370.82000000000005</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>301.06900000000002</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="0"/>
+        <v>238.298</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>182.50700000000001</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="0"/>
+        <v>162.14500000000001</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="0"/>
+        <v>133.696</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>107.75980000000001</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="0"/>
+        <v>91.865000000000009</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="0"/>
+        <v>77.087000000000003</v>
+      </c>
+      <c r="P3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R3">
+        <f>$B$1+$B$2*(72*R2+12*R2^2)+$B$3*10*R2</f>
+        <v>999.97500000000002</v>
+      </c>
+      <c r="S3">
+        <f t="shared" ref="S3:AA3" si="1">$B$1+$B$2*(72*S2+12*S2^2)+$B$3*10*S2</f>
+        <v>805.33100000000002</v>
+      </c>
+      <c r="T3">
+        <f t="shared" si="1"/>
+        <v>631.62699999999995</v>
+      </c>
+      <c r="U3">
+        <f t="shared" si="1"/>
+        <v>478.86299999999994</v>
+      </c>
+      <c r="V3">
+        <f t="shared" si="1"/>
+        <v>347.03899999999999</v>
+      </c>
+      <c r="W3">
+        <f t="shared" si="1"/>
+        <v>300.17259999999999</v>
+      </c>
+      <c r="X3">
+        <f t="shared" si="1"/>
+        <v>236.155</v>
+      </c>
+      <c r="Y3">
+        <f t="shared" si="1"/>
+        <v>179.67580000000001</v>
+      </c>
+      <c r="Z3">
+        <f t="shared" si="1"/>
+        <v>146.21100000000001</v>
+      </c>
+      <c r="AA3">
+        <f t="shared" si="1"/>
+        <v>116.0966</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE3">
+        <f>$B$1+$B$2*(76*AE2+20*AE2^2)+$B$3*15*AE2</f>
+        <v>1552.3989999999999</v>
+      </c>
+      <c r="AF3">
+        <f t="shared" ref="AF3:AN3" si="2">$B$1+$B$2*(76*AF2+20*AF2^2)+$B$3*15*AF2</f>
+        <v>1239.8420000000001</v>
+      </c>
+      <c r="AG3">
+        <f t="shared" si="2"/>
+        <v>962.18500000000006</v>
+      </c>
+      <c r="AH3">
+        <f t="shared" si="2"/>
+        <v>719.428</v>
+      </c>
+      <c r="AI3">
+        <f t="shared" si="2"/>
+        <v>511.57099999999997</v>
+      </c>
+      <c r="AJ3">
+        <f t="shared" si="2"/>
+        <v>438.2002</v>
+      </c>
+      <c r="AK3">
+        <f t="shared" si="2"/>
+        <v>338.61400000000003</v>
+      </c>
+      <c r="AL3">
+        <f t="shared" si="2"/>
+        <v>251.59180000000001</v>
+      </c>
+      <c r="AM3">
+        <f t="shared" si="2"/>
+        <v>200.55700000000002</v>
+      </c>
+      <c r="AN3">
+        <f t="shared" si="2"/>
+        <v>155.1062</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1000</v>
+      </c>
+      <c r="P4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q4">
+        <v>1000</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD4">
+        <v>1000</v>
+      </c>
+      <c r="AE4" s="7"/>
+      <c r="AF4" s="7"/>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>750</v>
+      </c>
+      <c r="Q5">
+        <v>750</v>
+      </c>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="AD5">
+        <v>750</v>
+      </c>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="7"/>
+      <c r="AG5" s="7"/>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>500</v>
+      </c>
+      <c r="Q6">
+        <v>500</v>
+      </c>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="AD6">
+        <v>500</v>
+      </c>
+      <c r="AE6" s="7"/>
+      <c r="AF6" s="7"/>
+      <c r="AG6" s="7"/>
+      <c r="AH6" s="7"/>
+      <c r="AI6" s="7"/>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>400</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="Q7">
+        <v>400</v>
+      </c>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="AD7">
+        <v>400</v>
+      </c>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="7"/>
+      <c r="AG7" s="7"/>
+      <c r="AH7" s="7"/>
+      <c r="AI7" s="7"/>
+      <c r="AJ7" s="7"/>
+    </row>
+    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>300</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="Q8">
+        <v>300</v>
+      </c>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="AD8">
+        <v>300</v>
+      </c>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="7"/>
+      <c r="AG8" s="7"/>
+      <c r="AH8" s="7"/>
+      <c r="AI8" s="7"/>
+      <c r="AJ8" s="7"/>
+      <c r="AK8" s="7"/>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>200</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="Q9">
+        <v>200</v>
+      </c>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="AD9">
+        <v>200</v>
+      </c>
+      <c r="AE9" s="7"/>
+      <c r="AF9" s="7"/>
+      <c r="AG9" s="7"/>
+      <c r="AH9" s="7"/>
+      <c r="AI9" s="7"/>
+      <c r="AJ9" s="7"/>
+      <c r="AK9" s="7"/>
+      <c r="AL9" s="7"/>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>100</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="Q10">
+        <v>100</v>
+      </c>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="7"/>
+      <c r="AA10" s="7"/>
+      <c r="AD10">
+        <v>100</v>
+      </c>
+      <c r="AE10" s="7"/>
+      <c r="AF10" s="7"/>
+      <c r="AG10" s="7"/>
+      <c r="AH10" s="7"/>
+      <c r="AI10" s="7"/>
+      <c r="AJ10" s="7"/>
+      <c r="AK10" s="7"/>
+      <c r="AL10" s="7"/>
+      <c r="AM10" s="7"/>
+      <c r="AN10" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
state from LSTM experiment
</commit_message>
<xml_diff>
--- a/python training environment/cRIO timing and SNR.xlsx
+++ b/python training environment/cRIO timing and SNR.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580" activeTab="2"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580"/>
   </bookViews>
   <sheets>
     <sheet name="experimental timing" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
   <si>
     <t>analog read</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>3 Cells</t>
+  </si>
+  <si>
+    <t>2 Cells</t>
   </si>
 </sst>
 </file>
@@ -322,11 +325,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="207379456"/>
-        <c:axId val="207381632"/>
+        <c:axId val="218848256"/>
+        <c:axId val="218850432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="207379456"/>
+        <c:axId val="218848256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -423,12 +426,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="207381632"/>
+        <c:crossAx val="218850432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="207381632"/>
+        <c:axId val="218850432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -525,7 +528,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="207379456"/>
+        <c:crossAx val="218848256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1157,7 +1160,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E169A768-9466-F90E-6327-3BB1745B7045}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E169A768-9466-F90E-6327-3BB1745B7045}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1467,7 +1470,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1477,7 +1480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -2387,8 +2390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView topLeftCell="Y1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AJ22" sqref="AJ22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2410,7 +2413,7 @@
         <v>29</v>
       </c>
       <c r="Q1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="AD1" t="s">
         <v>30</v>

</xml_diff>